<commit_message>
initial creation of the Branch v1.3.1
</commit_message>
<xml_diff>
--- a/_Additional Files/Datamodel/Datenmodel_Aktivgeschäft.xlsx
+++ b/_Additional Files/Datamodel/Datenmodel_Aktivgeschäft.xlsx
@@ -1,23 +1,24 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27928"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\SDK Projekte\Geno_Aktivgeschäft\_Additional Files\Datamodel\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\SmartAnalyzer.dev\GA_1.3.1\_Additional Files\Datamodel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{36FC7AB9-2DF8-4013-B155-C3793DC30C31}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EB8A6522-0183-4716-AEC0-0307BA9E2BFD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{DD12C30B-3E06-4062-9948-A95C3F6F8C93}"/>
+    <workbookView xWindow="22932" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{DD12C30B-3E06-4062-9948-A95C3F6F8C93}"/>
   </bookViews>
   <sheets>
     <sheet name="Übersicht" sheetId="2" r:id="rId1"/>
     <sheet name="KRM" sheetId="1" r:id="rId2"/>
     <sheet name="Kreditbeschlussbuch" sheetId="3" r:id="rId3"/>
     <sheet name="Schufa Negativmerkmale" sheetId="4" r:id="rId4"/>
-    <sheet name="Datenaufbereitung" sheetId="5" r:id="rId5"/>
+    <sheet name="Sicherheiten" sheetId="6" r:id="rId5"/>
+    <sheet name="Datenaufbereitung" sheetId="5" r:id="rId6"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -40,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="523" uniqueCount="183">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1353" uniqueCount="325">
   <si>
     <t>dd.mm.2021</t>
   </si>
@@ -590,13 +591,439 @@
   </si>
   <si>
     <t>Datensätze aus der Datei mit ENGA und PERS Datensätzen untereinander hängen.</t>
+  </si>
+  <si>
+    <t>Quelltabelle</t>
+  </si>
+  <si>
+    <t>Feldname in IDEA</t>
+  </si>
+  <si>
+    <t>Hinweis</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[Kreditsicherheit] </t>
+  </si>
+  <si>
+    <t>[Kunde]</t>
+  </si>
+  <si>
+    <t>NACHNAME_KURZ</t>
+  </si>
+  <si>
+    <t>SICHERHEITENNUMMER</t>
+  </si>
+  <si>
+    <t>STATUS_BEARBEITUNG</t>
+  </si>
+  <si>
+    <t>STATUS_SATZART</t>
+  </si>
+  <si>
+    <t>SICHERHEITENART</t>
+  </si>
+  <si>
+    <t>SICHERHEITENKATEGORIE</t>
+  </si>
+  <si>
+    <t>SICHERHEITENART_BEZEICHNUNG</t>
+  </si>
+  <si>
+    <t>DIE_QUALITATIVEN_ANFORDERUNGEN_SIND_ERFÜ</t>
+  </si>
+  <si>
+    <t>DIE_QUALITATIVEN_ANFORDERUNGEN_FÜR_DIE_G</t>
+  </si>
+  <si>
+    <t>RECHTSWIRKSAMKEITSDATUM</t>
+  </si>
+  <si>
+    <t>SICHERHEITENWERT_VERTEILT_JURISTISCH</t>
+  </si>
+  <si>
+    <t>[Kreditsicherheit].[Vermögenswertdaten]</t>
+  </si>
+  <si>
+    <t>BELEIHUNGSWERT</t>
+  </si>
+  <si>
+    <t>BELEIHUNGSGRENZE_ALS_BETRAG</t>
+  </si>
+  <si>
+    <t>BELEIHUNGSGRENZE_IN_PROZENT</t>
+  </si>
+  <si>
+    <t>NACHGEWIESENER_WERT</t>
+  </si>
+  <si>
+    <t>NACHGEWIESENER_WERT_PER</t>
+  </si>
+  <si>
+    <t>[Immobilie]</t>
+  </si>
+  <si>
+    <t>EIGENTÜMER_PERSONENNUMMER</t>
+  </si>
+  <si>
+    <t>IMMOBILIEN_NR</t>
+  </si>
+  <si>
+    <t>FEUERVERSICHERUNGSSCHEIN_NR</t>
+  </si>
+  <si>
+    <t>BEWERTUNGSART</t>
+  </si>
+  <si>
+    <t>BELEIHUNGSWERT_PER</t>
+  </si>
+  <si>
+    <t>BELEIHUNGSWERT_STATUS</t>
+  </si>
+  <si>
+    <t>BELEIHUNGSWERT_STATUS_PER</t>
+  </si>
+  <si>
+    <t>BELEIHUNGSWERT_STATUS_VON</t>
+  </si>
+  <si>
+    <t>BELEIHUNGSWERT_STATUS_NUMMER_DES_BEDIENE</t>
+  </si>
+  <si>
+    <t>BELEIHUNGSWERT_WURDE_ÜBERPRÜFT_AM</t>
+  </si>
+  <si>
+    <t>BELEIHUNGSWERT_WURDE_ÜBERPRÜFT_VON</t>
+  </si>
+  <si>
+    <t>BELEIHUNGSGRENZE_IN_EURO</t>
+  </si>
+  <si>
+    <t>NUTZUNG</t>
+  </si>
+  <si>
+    <t>NUTZUNGSART</t>
+  </si>
+  <si>
+    <t>OBJEKTART</t>
+  </si>
+  <si>
+    <t>OBJEKTART_BEZEICHNUNG</t>
+  </si>
+  <si>
+    <t>BÜRGSCHAFTSBETRAG</t>
+  </si>
+  <si>
+    <t>VERFÜGBARER_SICHERUNGSWERT</t>
+  </si>
+  <si>
+    <t>VERFÜGBARER_SICHERUNGSWERT_PER</t>
+  </si>
+  <si>
+    <t>[Zweckerklärung-Sicherheitenverteilung]</t>
+  </si>
+  <si>
+    <t>PERSONENNUMMER_SICHERHEITENGEBER</t>
+  </si>
+  <si>
+    <t>PERSONENNUMMER_SICHERHEITENNEHMER</t>
+  </si>
+  <si>
+    <t>SICHERHEITENUNTERNUMMER</t>
+  </si>
+  <si>
+    <t>KONTONUMMER_SICHERHEITENNEHMER</t>
+  </si>
+  <si>
+    <t>LETZTE_BERECHNUNG</t>
+  </si>
+  <si>
+    <t>ANTEIL_SICHERUNGSWERT_GEMÄß_BERECHNUNGSA</t>
+  </si>
+  <si>
+    <t>SICHERUNGSWERT_AUF_BASIS_VON</t>
+  </si>
+  <si>
+    <t>TYP_DES_SICHERUNGSWERTES</t>
+  </si>
+  <si>
+    <t>EINZELRATING</t>
+  </si>
+  <si>
+    <t>RISIKOSTATUS_MARISK_SEIT</t>
+  </si>
+  <si>
+    <t>Personennummer</t>
+  </si>
+  <si>
+    <t>Nachname kurz</t>
+  </si>
+  <si>
+    <t>Sicherheitennummer</t>
+  </si>
+  <si>
+    <t>Sicherheitenart</t>
+  </si>
+  <si>
+    <t>Sicherheitenkategorie</t>
+  </si>
+  <si>
+    <t>Rechtswirksamkeitsdatum</t>
+  </si>
+  <si>
+    <t>Beleihungswert</t>
+  </si>
+  <si>
+    <t>Status Bearbeitung</t>
+  </si>
+  <si>
+    <t>Status Satzart</t>
+  </si>
+  <si>
+    <t>Sicherheitenart Bezeichnung</t>
+  </si>
+  <si>
+    <t>Die qualitativen Anforderungen sind erfüllt</t>
+  </si>
+  <si>
+    <t>Die qualitativen Anforderungen für die GroMiKV sind erfüllt</t>
+  </si>
+  <si>
+    <t>Sicherheitenwert verteilt juristisch</t>
+  </si>
+  <si>
+    <t>Beleihungsgrenze als Betrag</t>
+  </si>
+  <si>
+    <t>Beleihungsgrenze in Prozent</t>
+  </si>
+  <si>
+    <t>Nachgewiesener Wert</t>
+  </si>
+  <si>
+    <t>Nachgewiesener Wert per</t>
+  </si>
+  <si>
+    <t>EINGETRAGENER_BETRAG</t>
+  </si>
+  <si>
+    <t>Eingetragener betrag</t>
+  </si>
+  <si>
+    <t>Eigentümer Personennummer</t>
+  </si>
+  <si>
+    <t>Immobilien-Nr.</t>
+  </si>
+  <si>
+    <t>Feuerversicherungsschein Nr.</t>
+  </si>
+  <si>
+    <t>Bewertungsart</t>
+  </si>
+  <si>
+    <t>Beleihungswert per</t>
+  </si>
+  <si>
+    <t>Beleihungswert Status</t>
+  </si>
+  <si>
+    <t>Beleihungswert Status per</t>
+  </si>
+  <si>
+    <t>Beleihungswert Status von</t>
+  </si>
+  <si>
+    <t>Beleihungswert Status Nummer des Bedieners</t>
+  </si>
+  <si>
+    <t>Beleihungswert wurde überprüft am</t>
+  </si>
+  <si>
+    <t>Beleihungswert wurde überprüft von</t>
+  </si>
+  <si>
+    <t>Beleihungsgrenze in Euro</t>
+  </si>
+  <si>
+    <t>Nutzung</t>
+  </si>
+  <si>
+    <t>Nutzungsart</t>
+  </si>
+  <si>
+    <t>Objektart</t>
+  </si>
+  <si>
+    <t>Objektart Bezeichnung</t>
+  </si>
+  <si>
+    <t>Bürgschaftsbetrag</t>
+  </si>
+  <si>
+    <t>Verfügbarer Sicherungswert</t>
+  </si>
+  <si>
+    <t>Verfügbarer Sicherungswert per</t>
+  </si>
+  <si>
+    <t>Personennummer Sicherheitengeber</t>
+  </si>
+  <si>
+    <t>Personennummer Sicherheitennehmer</t>
+  </si>
+  <si>
+    <t>Sicherheitenunternummer</t>
+  </si>
+  <si>
+    <t>Kontonummer Sicherheitennehmer</t>
+  </si>
+  <si>
+    <t>Letzte Berechnung</t>
+  </si>
+  <si>
+    <t>Anteil Sicherungswert gemäß Berechnungsart und Typ</t>
+  </si>
+  <si>
+    <t>Sicherungswert auf Basis von</t>
+  </si>
+  <si>
+    <t>Typ des Sicherungswertes</t>
+  </si>
+  <si>
+    <t>Einzelrating</t>
+  </si>
+  <si>
+    <t>Risikostatus MaRisk</t>
+  </si>
+  <si>
+    <t>Risikostatus MaRisk seit</t>
+  </si>
+  <si>
+    <t>Kundenberater</t>
+  </si>
+  <si>
+    <t>Si-Basisdaten-Immo verknüpft mit Sicherheiten-Zweckerklärungen-Si-Wert</t>
+  </si>
+  <si>
+    <t>Si-Basisdaten verknüpft mit Sicherheiten-Zweckerklärungen-Si-Wert</t>
+  </si>
+  <si>
+    <t>Alle Datensätze der "Sicherheiten-Basisdaten" (einschließlich aller Felder) werden mit der Tabelle "Sicherheiten-Zweckerklärungen-Si-Wert" (einschließlich der beiden Felder "Risikostatus MaRisk" und "Risikostatus MaRisk seit") verknüpft. Die Personennummer der Sicherheitengeber und die Sicherheitennummer dienen als Schlüsselfelder.</t>
+  </si>
+  <si>
+    <t>Alle Datensätze der "Sicherheiten-Basisdaten-Immo" (einschließlich aller Felder) werden mit der Tabelle "Sicherheiten-Zweckerklärungen-Si-Wert" (einschließlich der beiden Felder "Risikostatus MaRisk" und "Risikostatus MaRisk seit") verknüpft. Die Personennummer der Sicherheitengeber und die Sicherheitennummer dienen als Schlüsselfelder.</t>
+  </si>
+  <si>
+    <t>Die neu erstellte Tabelle aus Schritt 1 wird mit der Tabelle "Sicherheiten-Basisdaten-Immo" verknüpft. Die Personennummer der Sicherheitengeber und die Sicherheitennummer dienen als Schlüsselfelder.</t>
+  </si>
+  <si>
+    <t>Die Tabellen "Sicherheiten-Basisdaten", "Sicherheiten-Basisdaten-Immo" und "Sicherheiten-Bürgschaften-Haftungsfreistellungen" sind angehängt (einschließlich der Felder: Personennummer, Nachname kurz, Sicherheitenart, Sicherheitenart Bezeichnung und Sicherheitenwert verteilt juristisch)</t>
+  </si>
+  <si>
+    <t>Die Summe der "Sicherheitenwert verteilt juristisch" je "Sicherheitenart" wurde berechnet.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Hinzufügen eines berechneten Feldes zur "Sicherheiten-Zweckerklärungen-Realkredit": Summe aus dem Feld "Anteil Sicherungswert gemäß Berechnungsart und Typ" für die jeweilige "Personen Nr. Sicherheitennehmer" </t>
+  </si>
+  <si>
+    <t>{Sicherheiten-Basisdaten}</t>
+  </si>
+  <si>
+    <t>{Sicherheiten-Basisdaten-Immo}</t>
+  </si>
+  <si>
+    <t>{Sicherheiten-Bürgschaften-Haftungsfreistellungen}</t>
+  </si>
+  <si>
+    <t>{Sicherheiten-Zweckerklärungen-Realkredit}</t>
+  </si>
+  <si>
+    <t>{Sicherheiten-Zweckerklärungen-Si-Wert}</t>
+  </si>
+  <si>
+    <t>SICHERHEITENKATEGORIE_BEZEICHNUNG</t>
+  </si>
+  <si>
+    <t>BEWERTUNGSART_BEZEICHNUNG</t>
+  </si>
+  <si>
+    <t>BELEIHUNGSWERT_STATUS_BEZEICHNUNG</t>
+  </si>
+  <si>
+    <t>NUTZUNG_BEZEICHNUNG</t>
+  </si>
+  <si>
+    <t>NUTZUNGSART_BEZEICHNUNG</t>
+  </si>
+  <si>
+    <t>SICHERUNGSWERT_AUF_BASIS_VON_BEZEICHNUNG</t>
+  </si>
+  <si>
+    <t>TYP_DES_SICHERUNGSWERTES_BEZEICHNUNG</t>
+  </si>
+  <si>
+    <t>RISIKOSTATUS_MARISK_BEZEICHNUNG</t>
+  </si>
+  <si>
+    <t>{Codes und Bezeichnungen aus den Sicherheiten}</t>
+  </si>
+  <si>
+    <t>Sicherheiten</t>
+  </si>
+  <si>
+    <t>Basisdaten mit Immobilien und Bürgschaften angehängt-Sicherheitenwert je Sicherheitenart summiert</t>
+  </si>
+  <si>
+    <t>SUMME_SI_WERT_JE_SICHERHEITENNEHMER</t>
+  </si>
+  <si>
+    <t>Zweckerklärungen Realkredit verknüpft mit Basisdaten-Immo</t>
+  </si>
+  <si>
+    <t>ANZ_SAETZE</t>
+  </si>
+  <si>
+    <t>SICHERHEITENWERT_VERTEILT_JURISTISCH_SUM</t>
+  </si>
+  <si>
+    <t>Das Bezeichnungsfeld SICHERHEITENKATEGORIE_BEZEICHNUNG aus der Tabelle {Codes und Bezeichnungen aus den Sicherheiten} wurde hinzugefügt.</t>
+  </si>
+  <si>
+    <t>Die Bezeichnungsfelder BEWERTUNGSART_BEZEICHNUNG, BELEIHUNGSWERT_STATUS_BEZEICHNUNG, NUTZUNG_BEZEICHNUNG und NUTZUNGSART_BEZEICHNUNG aus der Tabelle {Codes und Bezeichnungen aus den Sicherheiten} wurden hinzugefügt.</t>
+  </si>
+  <si>
+    <t>Die Bezeichnungsfelder SICHERUNGSWERT_AUF_BASIS_VON_BEZEICHNUNG, TYP_DES_SICHERUNGSWERTES_BEZEICHNUNG und RISIKOSTATUS_MARISK_BEZEICHNUNG aus der Tabelle {Codes und Bezeichnungen aus den Sicherheiten} wurden hinzugefügt.</t>
+  </si>
+  <si>
+    <t>{Sicherheiten_Basisdaten}_mit Bezeichnungen</t>
+  </si>
+  <si>
+    <t>{Sicherheiten-Basisdaten-Immo}_mit Bezeichnungen</t>
+  </si>
+  <si>
+    <t>{Sicherheiten_Bürgschaften_Haftungsfreistellungen}_mit Bezeichnungen</t>
+  </si>
+  <si>
+    <t>{Sicherheiten-Zweckerklärungen-Realkredit}_mit Bezeichnungen</t>
+  </si>
+  <si>
+    <t>{Sicherheiten-Zweckerklärungen-Si-Wert}_mit Bezeichnungen</t>
+  </si>
+  <si>
+    <t>SICHERHEITENARTENSCHLÜSSEL</t>
+  </si>
+  <si>
+    <t>SICHERHEITENARTENBEZEICHNUNG</t>
+  </si>
+  <si>
+    <t>{Sicherheitenartenschlüssel mit Bezeichnung}</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4">
+  <fonts count="5">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -623,6 +1050,12 @@
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Docs-Calibri"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Aptos"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="5">
@@ -723,7 +1156,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
@@ -734,6 +1167,13 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
@@ -743,20 +1183,50 @@
     <xf numFmtId="14" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Link" xfId="1" builtinId="8"/>
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="6">
+  <dxfs count="8">
     <dxf>
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Aptos"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Aptos"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
     </dxf>
     <dxf>
       <font>
@@ -886,11 +1356,11 @@
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{025F6466-0983-4E03-BD21-E36E2D4BB135}" name="Tabelle3" displayName="Tabelle3" ref="C2:D95" totalsRowShown="0" headerRowDxfId="5" dataDxfId="4" tableBorderDxfId="3">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{025F6466-0983-4E03-BD21-E36E2D4BB135}" name="Tabelle3" displayName="Tabelle3" ref="C2:D95" totalsRowShown="0" headerRowDxfId="7" dataDxfId="6" tableBorderDxfId="5">
   <autoFilter ref="C2:D95" xr:uid="{025F6466-0983-4E03-BD21-E36E2D4BB135}"/>
   <tableColumns count="2">
-    <tableColumn id="1" xr3:uid="{30B239BA-9949-420A-98E8-8B265B9803AB}" name="Feldname" dataDxfId="2"/>
-    <tableColumn id="2" xr3:uid="{33C6FC88-E9DD-46BB-9DC4-8CCB9FE2FF01}" name="Feldtyp" dataDxfId="1"/>
+    <tableColumn id="1" xr3:uid="{30B239BA-9949-420A-98E8-8B265B9803AB}" name="Feldname" dataDxfId="4"/>
+    <tableColumn id="2" xr3:uid="{33C6FC88-E9DD-46BB-9DC4-8CCB9FE2FF01}" name="Feldtyp" dataDxfId="3"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium3" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -919,8 +1389,23 @@
 </file>
 
 <file path=xl/tables/table6.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{AFBD5704-4365-4CD0-B244-1DE463EAAD36}" name="Tabelle6" displayName="Tabelle6" ref="A1:C4" totalsRowShown="0">
-  <autoFilter ref="A1:C4" xr:uid="{AFBD5704-4365-4CD0-B244-1DE463EAAD36}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="7" xr:uid="{F4DC95B3-5A93-4E83-822A-D2F28CEF61DB}" name="Tabelle2268" displayName="Tabelle2268" ref="A1:F210" totalsRowShown="0">
+  <autoFilter ref="A1:F210" xr:uid="{F4DC95B3-5A93-4E83-822A-D2F28CEF61DB}"/>
+  <tableColumns count="6">
+    <tableColumn id="1" xr3:uid="{B636E722-D4E1-4EC3-989F-0D7F1A83E3A9}" name="Tabelle"/>
+    <tableColumn id="6" xr3:uid="{50962C8D-1782-4B80-A009-59DC4B953006}" name="Feldname"/>
+    <tableColumn id="4" xr3:uid="{EAAD599C-6478-43F7-BBCD-942775823593}" name="Quelltabelle" dataDxfId="2"/>
+    <tableColumn id="2" xr3:uid="{0C85A38F-AD9E-4AB1-8260-AECBC10040F7}" name="Feldtyp" dataDxfId="1"/>
+    <tableColumn id="3" xr3:uid="{C211D8DC-506D-4446-9DDC-DAC745976D34}" name="Feldname in IDEA"/>
+    <tableColumn id="5" xr3:uid="{1263A1D6-BBAE-4CEF-9564-4F990EA30031}" name="Hinweis"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table7.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{AFBD5704-4365-4CD0-B244-1DE463EAAD36}" name="Tabelle6" displayName="Tabelle6" ref="A1:C15" totalsRowShown="0">
+  <autoFilter ref="A1:C15" xr:uid="{AFBD5704-4365-4CD0-B244-1DE463EAAD36}"/>
   <tableColumns count="3">
     <tableColumn id="1" xr3:uid="{0040EB4B-9824-4164-BB4F-ACD9E12BBA5B}" name="Tabelle"/>
     <tableColumn id="2" xr3:uid="{8F8CB15B-E551-4E39-B634-6DB8D56F0823}" name="Schritt"/>
@@ -931,9 +1416,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 – 2022-Design">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 – 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -971,7 +1456,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 – 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -1077,7 +1562,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 – 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -1219,7 +1704,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1227,14 +1712,14 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7D49AAF5-C7BE-4E76-885B-1467FFF687CC}">
-  <dimension ref="A1:B15"/>
+  <dimension ref="A1:B16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4"/>
   <cols>
     <col min="1" max="1" width="44.44140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="50.88671875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="50.77734375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" ht="25.8">
@@ -1314,11 +1799,17 @@
         <v>115</v>
       </c>
     </row>
+    <row r="16" spans="1:2">
+      <c r="A16" s="5" t="s">
+        <v>308</v>
+      </c>
+    </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="A13" location="KRM!A1" display="KRM" xr:uid="{8DD138AA-6B69-4CA1-982E-873D90CF6260}"/>
     <hyperlink ref="A14" location="Kreditbeschlussbuch!A1" display="Kreditbeschlussbuch" xr:uid="{0CF7D835-B897-431C-97D3-E75B0C5266D7}"/>
     <hyperlink ref="A15" location="'Schufa Negativmerkmale'!A1" display="Schufa Negativmerkmale" xr:uid="{253B4C77-9FDB-47EF-89C8-7BF9D1642B17}"/>
+    <hyperlink ref="A16" location="Sicherheiten!A1" display="Sicherheiten" xr:uid="{DB770FA9-17B8-45FF-94BC-A5EE16637D06}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -1345,14 +1836,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4">
-      <c r="A1" s="10" t="s">
+      <c r="A1" s="13" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="10"/>
-      <c r="C1" s="11">
+      <c r="B1" s="13"/>
+      <c r="C1" s="14">
         <v>44698</v>
       </c>
-      <c r="D1" s="11"/>
+      <c r="D1" s="14"/>
     </row>
     <row r="2" spans="1:4">
       <c r="A2" t="s">
@@ -2635,13 +3126,13 @@
         <v>92</v>
       </c>
       <c r="B94" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="C94" s="3" t="s">
         <v>92</v>
       </c>
       <c r="D94" s="4" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
     </row>
     <row r="95" spans="1:4">
@@ -2681,15 +3172,15 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="42.88671875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="42.77734375" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="13.44140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2">
-      <c r="A1" s="12">
+      <c r="A1" s="15">
         <v>45145</v>
       </c>
-      <c r="B1" s="10"/>
+      <c r="B1" s="13"/>
     </row>
     <row r="2" spans="1:2">
       <c r="A2" t="s">
@@ -2923,20 +3414,20 @@
   <dimension ref="A1:B36"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:B2"/>
+      <selection sqref="A1:B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="47.88671875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="47.77734375" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="13.44140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2">
-      <c r="A1" s="12">
+      <c r="A1" s="15">
         <v>45145</v>
       </c>
-      <c r="B1" s="10"/>
+      <c r="B1" s="13"/>
     </row>
     <row r="2" spans="1:2">
       <c r="A2" t="s">
@@ -3230,16 +3721,2973 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DF424794-3269-4271-90B8-7AD6608D0FA6}">
-  <dimension ref="A1:Q4"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{64BBF3ED-6AE3-41E7-8C4D-B521F3F27022}">
+  <dimension ref="A1:F210"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="18.88671875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="86.5546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="49.77734375" customWidth="1"/>
+    <col min="3" max="3" width="42.21875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14" customWidth="1"/>
+    <col min="5" max="5" width="47.77734375" customWidth="1"/>
+    <col min="6" max="6" width="16.5546875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="20.21875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6">
+      <c r="A1" t="s">
+        <v>177</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>183</v>
+      </c>
+      <c r="D1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" t="s">
+        <v>184</v>
+      </c>
+      <c r="F1" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6">
+      <c r="A2" t="s">
+        <v>307</v>
+      </c>
+      <c r="C2" s="12"/>
+      <c r="D2" t="s">
+        <v>95</v>
+      </c>
+      <c r="E2" t="s">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6">
+      <c r="A3" t="s">
+        <v>307</v>
+      </c>
+      <c r="C3" s="12"/>
+      <c r="D3" t="s">
+        <v>95</v>
+      </c>
+      <c r="E3" t="s">
+        <v>299</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6">
+      <c r="A4" t="s">
+        <v>307</v>
+      </c>
+      <c r="C4" s="12"/>
+      <c r="D4" t="s">
+        <v>95</v>
+      </c>
+      <c r="E4" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6">
+      <c r="A5" t="s">
+        <v>307</v>
+      </c>
+      <c r="C5" s="12"/>
+      <c r="D5" t="s">
+        <v>95</v>
+      </c>
+      <c r="E5" t="s">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6">
+      <c r="A6" t="s">
+        <v>307</v>
+      </c>
+      <c r="C6" s="12"/>
+      <c r="D6" t="s">
+        <v>95</v>
+      </c>
+      <c r="E6" t="s">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6">
+      <c r="A7" t="s">
+        <v>307</v>
+      </c>
+      <c r="C7" s="12"/>
+      <c r="D7" t="s">
+        <v>95</v>
+      </c>
+      <c r="E7" t="s">
+        <v>301</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6">
+      <c r="A8" t="s">
+        <v>307</v>
+      </c>
+      <c r="C8" s="12"/>
+      <c r="D8" t="s">
+        <v>95</v>
+      </c>
+      <c r="E8" t="s">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6">
+      <c r="A9" t="s">
+        <v>307</v>
+      </c>
+      <c r="C9" s="12"/>
+      <c r="D9" t="s">
+        <v>95</v>
+      </c>
+      <c r="E9" t="s">
+        <v>302</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6">
+      <c r="A10" t="s">
+        <v>307</v>
+      </c>
+      <c r="C10" s="12"/>
+      <c r="D10" t="s">
+        <v>95</v>
+      </c>
+      <c r="E10" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6">
+      <c r="A11" t="s">
+        <v>307</v>
+      </c>
+      <c r="C11" s="12"/>
+      <c r="D11" t="s">
+        <v>95</v>
+      </c>
+      <c r="E11" t="s">
+        <v>303</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6">
+      <c r="A12" t="s">
+        <v>307</v>
+      </c>
+      <c r="C12" s="12"/>
+      <c r="D12" t="s">
+        <v>95</v>
+      </c>
+      <c r="E12" t="s">
+        <v>232</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6">
+      <c r="A13" t="s">
+        <v>307</v>
+      </c>
+      <c r="C13" s="12"/>
+      <c r="D13" t="s">
+        <v>95</v>
+      </c>
+      <c r="E13" t="s">
+        <v>304</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6">
+      <c r="A14" t="s">
+        <v>307</v>
+      </c>
+      <c r="C14" s="12"/>
+      <c r="D14" t="s">
+        <v>95</v>
+      </c>
+      <c r="E14" t="s">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6">
+      <c r="A15" t="s">
+        <v>307</v>
+      </c>
+      <c r="C15" s="12"/>
+      <c r="D15" t="s">
+        <v>95</v>
+      </c>
+      <c r="E15" t="s">
+        <v>305</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6">
+      <c r="A16" t="s">
+        <v>307</v>
+      </c>
+      <c r="C16" s="12"/>
+      <c r="D16" t="s">
+        <v>95</v>
+      </c>
+      <c r="E16" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5">
+      <c r="A17" t="s">
+        <v>307</v>
+      </c>
+      <c r="C17" s="12"/>
+      <c r="D17" t="s">
+        <v>95</v>
+      </c>
+      <c r="E17" t="s">
+        <v>306</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5">
+      <c r="A18" t="s">
+        <v>294</v>
+      </c>
+      <c r="B18" t="s">
+        <v>236</v>
+      </c>
+      <c r="C18" s="12" t="s">
+        <v>186</v>
+      </c>
+      <c r="D18" t="s">
+        <v>95</v>
+      </c>
+      <c r="E18" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5">
+      <c r="A19" t="s">
+        <v>294</v>
+      </c>
+      <c r="B19" t="s">
+        <v>237</v>
+      </c>
+      <c r="C19" s="12" t="s">
+        <v>187</v>
+      </c>
+      <c r="D19" t="s">
+        <v>95</v>
+      </c>
+      <c r="E19" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5">
+      <c r="A20" t="s">
+        <v>294</v>
+      </c>
+      <c r="B20" t="s">
+        <v>238</v>
+      </c>
+      <c r="C20" s="12" t="s">
+        <v>186</v>
+      </c>
+      <c r="D20" t="s">
+        <v>95</v>
+      </c>
+      <c r="E20" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5">
+      <c r="A21" t="s">
+        <v>294</v>
+      </c>
+      <c r="B21" t="s">
+        <v>243</v>
+      </c>
+      <c r="C21" s="12" t="s">
+        <v>186</v>
+      </c>
+      <c r="D21" t="s">
+        <v>95</v>
+      </c>
+      <c r="E21" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5">
+      <c r="A22" t="s">
+        <v>294</v>
+      </c>
+      <c r="B22" t="s">
+        <v>244</v>
+      </c>
+      <c r="C22" s="12" t="s">
+        <v>186</v>
+      </c>
+      <c r="D22" t="s">
+        <v>95</v>
+      </c>
+      <c r="E22" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5">
+      <c r="A23" t="s">
+        <v>294</v>
+      </c>
+      <c r="B23" t="s">
+        <v>239</v>
+      </c>
+      <c r="C23" s="12" t="s">
+        <v>186</v>
+      </c>
+      <c r="D23" t="s">
+        <v>95</v>
+      </c>
+      <c r="E23" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5">
+      <c r="A24" t="s">
+        <v>294</v>
+      </c>
+      <c r="B24" t="s">
+        <v>240</v>
+      </c>
+      <c r="C24" s="12" t="s">
+        <v>186</v>
+      </c>
+      <c r="D24" t="s">
+        <v>95</v>
+      </c>
+      <c r="E24" t="s">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5">
+      <c r="A25" t="s">
+        <v>294</v>
+      </c>
+      <c r="B25" t="s">
+        <v>245</v>
+      </c>
+      <c r="C25" s="12" t="s">
+        <v>186</v>
+      </c>
+      <c r="D25" t="s">
+        <v>95</v>
+      </c>
+      <c r="E25" t="s">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5">
+      <c r="A26" t="s">
+        <v>294</v>
+      </c>
+      <c r="B26" t="s">
+        <v>246</v>
+      </c>
+      <c r="C26" s="12" t="s">
+        <v>186</v>
+      </c>
+      <c r="D26" t="s">
+        <v>95</v>
+      </c>
+      <c r="E26" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5">
+      <c r="A27" t="s">
+        <v>294</v>
+      </c>
+      <c r="B27" t="s">
+        <v>247</v>
+      </c>
+      <c r="C27" s="12" t="s">
+        <v>186</v>
+      </c>
+      <c r="D27" t="s">
+        <v>95</v>
+      </c>
+      <c r="E27" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5">
+      <c r="A28" t="s">
+        <v>294</v>
+      </c>
+      <c r="B28" t="s">
+        <v>241</v>
+      </c>
+      <c r="C28" s="12" t="s">
+        <v>186</v>
+      </c>
+      <c r="D28" t="s">
+        <v>96</v>
+      </c>
+      <c r="E28" t="s">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5">
+      <c r="A29" t="s">
+        <v>294</v>
+      </c>
+      <c r="B29" t="s">
+        <v>248</v>
+      </c>
+      <c r="C29" s="12" t="s">
+        <v>186</v>
+      </c>
+      <c r="D29" t="s">
+        <v>142</v>
+      </c>
+      <c r="E29" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5">
+      <c r="A30" t="s">
+        <v>294</v>
+      </c>
+      <c r="B30" t="s">
+        <v>242</v>
+      </c>
+      <c r="C30" s="12" t="s">
+        <v>199</v>
+      </c>
+      <c r="D30" t="s">
+        <v>142</v>
+      </c>
+      <c r="E30" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5">
+      <c r="A31" t="s">
+        <v>294</v>
+      </c>
+      <c r="B31" t="s">
+        <v>249</v>
+      </c>
+      <c r="C31" s="12" t="s">
+        <v>199</v>
+      </c>
+      <c r="D31" t="s">
+        <v>142</v>
+      </c>
+      <c r="E31" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5">
+      <c r="A32" t="s">
+        <v>294</v>
+      </c>
+      <c r="B32" t="s">
+        <v>250</v>
+      </c>
+      <c r="C32" s="12" t="s">
+        <v>199</v>
+      </c>
+      <c r="D32" t="s">
+        <v>142</v>
+      </c>
+      <c r="E32" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5">
+      <c r="A33" t="s">
+        <v>294</v>
+      </c>
+      <c r="B33" t="s">
+        <v>251</v>
+      </c>
+      <c r="C33" s="12" t="s">
+        <v>199</v>
+      </c>
+      <c r="D33" t="s">
+        <v>142</v>
+      </c>
+      <c r="E33" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5">
+      <c r="A34" t="s">
+        <v>294</v>
+      </c>
+      <c r="B34" t="s">
+        <v>252</v>
+      </c>
+      <c r="C34" s="12" t="s">
+        <v>199</v>
+      </c>
+      <c r="D34" t="s">
+        <v>96</v>
+      </c>
+      <c r="E34" t="s">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5">
+      <c r="A35" t="s">
+        <v>295</v>
+      </c>
+      <c r="B35" t="s">
+        <v>236</v>
+      </c>
+      <c r="C35" s="12" t="s">
+        <v>186</v>
+      </c>
+      <c r="D35" t="s">
+        <v>95</v>
+      </c>
+      <c r="E35" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5">
+      <c r="A36" t="s">
+        <v>295</v>
+      </c>
+      <c r="B36" t="s">
+        <v>237</v>
+      </c>
+      <c r="C36" s="12" t="s">
+        <v>187</v>
+      </c>
+      <c r="D36" t="s">
+        <v>95</v>
+      </c>
+      <c r="E36" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5">
+      <c r="A37" t="s">
+        <v>295</v>
+      </c>
+      <c r="B37" t="s">
+        <v>238</v>
+      </c>
+      <c r="C37" s="12" t="s">
+        <v>186</v>
+      </c>
+      <c r="D37" t="s">
+        <v>95</v>
+      </c>
+      <c r="E37" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5">
+      <c r="A38" t="s">
+        <v>295</v>
+      </c>
+      <c r="B38" t="s">
+        <v>243</v>
+      </c>
+      <c r="C38" s="12" t="s">
+        <v>186</v>
+      </c>
+      <c r="D38" t="s">
+        <v>95</v>
+      </c>
+      <c r="E38" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="39" spans="1:5">
+      <c r="A39" t="s">
+        <v>295</v>
+      </c>
+      <c r="B39" t="s">
+        <v>244</v>
+      </c>
+      <c r="C39" s="12" t="s">
+        <v>186</v>
+      </c>
+      <c r="D39" t="s">
+        <v>95</v>
+      </c>
+      <c r="E39" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="40" spans="1:5">
+      <c r="A40" t="s">
+        <v>295</v>
+      </c>
+      <c r="B40" t="s">
+        <v>239</v>
+      </c>
+      <c r="C40" s="12" t="s">
+        <v>186</v>
+      </c>
+      <c r="D40" t="s">
+        <v>95</v>
+      </c>
+      <c r="E40" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="41" spans="1:5">
+      <c r="A41" t="s">
+        <v>295</v>
+      </c>
+      <c r="B41" t="s">
+        <v>254</v>
+      </c>
+      <c r="C41" s="12" t="s">
+        <v>205</v>
+      </c>
+      <c r="D41" t="s">
+        <v>142</v>
+      </c>
+      <c r="E41" t="s">
+        <v>253</v>
+      </c>
+    </row>
+    <row r="42" spans="1:5">
+      <c r="A42" t="s">
+        <v>295</v>
+      </c>
+      <c r="B42" t="s">
+        <v>245</v>
+      </c>
+      <c r="C42" s="12" t="s">
+        <v>186</v>
+      </c>
+      <c r="D42" t="s">
+        <v>95</v>
+      </c>
+      <c r="E42" t="s">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="43" spans="1:5">
+      <c r="A43" t="s">
+        <v>295</v>
+      </c>
+      <c r="B43" t="s">
+        <v>255</v>
+      </c>
+      <c r="C43" s="12" t="s">
+        <v>205</v>
+      </c>
+      <c r="D43" t="s">
+        <v>95</v>
+      </c>
+      <c r="E43" t="s">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="44" spans="1:5">
+      <c r="A44" t="s">
+        <v>295</v>
+      </c>
+      <c r="B44" t="s">
+        <v>256</v>
+      </c>
+      <c r="C44" s="12" t="s">
+        <v>205</v>
+      </c>
+      <c r="D44" t="s">
+        <v>95</v>
+      </c>
+      <c r="E44" t="s">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="45" spans="1:5">
+      <c r="A45" t="s">
+        <v>295</v>
+      </c>
+      <c r="B45" t="s">
+        <v>257</v>
+      </c>
+      <c r="C45" s="12" t="s">
+        <v>205</v>
+      </c>
+      <c r="D45" t="s">
+        <v>95</v>
+      </c>
+      <c r="E45" t="s">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="46" spans="1:5">
+      <c r="A46" t="s">
+        <v>295</v>
+      </c>
+      <c r="B46" t="s">
+        <v>258</v>
+      </c>
+      <c r="C46" s="12" t="s">
+        <v>205</v>
+      </c>
+      <c r="D46" t="s">
+        <v>95</v>
+      </c>
+      <c r="E46" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="47" spans="1:5">
+      <c r="A47" t="s">
+        <v>295</v>
+      </c>
+      <c r="B47" t="s">
+        <v>242</v>
+      </c>
+      <c r="C47" s="12" t="s">
+        <v>205</v>
+      </c>
+      <c r="D47" t="s">
+        <v>142</v>
+      </c>
+      <c r="E47" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="48" spans="1:5">
+      <c r="A48" t="s">
+        <v>295</v>
+      </c>
+      <c r="B48" t="s">
+        <v>259</v>
+      </c>
+      <c r="C48" s="12" t="s">
+        <v>205</v>
+      </c>
+      <c r="D48" t="s">
+        <v>96</v>
+      </c>
+      <c r="E48" t="s">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="49" spans="1:5">
+      <c r="A49" t="s">
+        <v>295</v>
+      </c>
+      <c r="B49" t="s">
+        <v>260</v>
+      </c>
+      <c r="C49" s="12" t="s">
+        <v>205</v>
+      </c>
+      <c r="D49" t="s">
+        <v>95</v>
+      </c>
+      <c r="E49" t="s">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="50" spans="1:5">
+      <c r="A50" t="s">
+        <v>295</v>
+      </c>
+      <c r="B50" t="s">
+        <v>261</v>
+      </c>
+      <c r="C50" s="12" t="s">
+        <v>205</v>
+      </c>
+      <c r="D50" t="s">
+        <v>96</v>
+      </c>
+      <c r="E50" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="51" spans="1:5">
+      <c r="A51" t="s">
+        <v>295</v>
+      </c>
+      <c r="B51" t="s">
+        <v>262</v>
+      </c>
+      <c r="C51" s="12" t="s">
+        <v>205</v>
+      </c>
+      <c r="D51" t="s">
+        <v>95</v>
+      </c>
+      <c r="E51" t="s">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="52" spans="1:5">
+      <c r="A52" t="s">
+        <v>295</v>
+      </c>
+      <c r="B52" t="s">
+        <v>263</v>
+      </c>
+      <c r="C52" s="12" t="s">
+        <v>205</v>
+      </c>
+      <c r="D52" t="s">
+        <v>95</v>
+      </c>
+      <c r="E52" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="53" spans="1:5">
+      <c r="A53" t="s">
+        <v>295</v>
+      </c>
+      <c r="B53" t="s">
+        <v>264</v>
+      </c>
+      <c r="C53" s="12" t="s">
+        <v>205</v>
+      </c>
+      <c r="D53" t="s">
+        <v>96</v>
+      </c>
+      <c r="E53" t="s">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="54" spans="1:5">
+      <c r="A54" t="s">
+        <v>295</v>
+      </c>
+      <c r="B54" t="s">
+        <v>265</v>
+      </c>
+      <c r="C54" s="12" t="s">
+        <v>205</v>
+      </c>
+      <c r="D54" t="s">
+        <v>95</v>
+      </c>
+      <c r="E54" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="55" spans="1:5">
+      <c r="A55" t="s">
+        <v>295</v>
+      </c>
+      <c r="B55" t="s">
+        <v>266</v>
+      </c>
+      <c r="C55" s="12" t="s">
+        <v>205</v>
+      </c>
+      <c r="D55" t="s">
+        <v>142</v>
+      </c>
+      <c r="E55" t="s">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="56" spans="1:5">
+      <c r="A56" t="s">
+        <v>295</v>
+      </c>
+      <c r="B56" t="s">
+        <v>250</v>
+      </c>
+      <c r="C56" s="12" t="s">
+        <v>205</v>
+      </c>
+      <c r="D56" t="s">
+        <v>142</v>
+      </c>
+      <c r="E56" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="57" spans="1:5">
+      <c r="A57" t="s">
+        <v>295</v>
+      </c>
+      <c r="B57" t="s">
+        <v>248</v>
+      </c>
+      <c r="C57" s="12" t="s">
+        <v>186</v>
+      </c>
+      <c r="D57" t="s">
+        <v>95</v>
+      </c>
+      <c r="E57" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="58" spans="1:5">
+      <c r="A58" t="s">
+        <v>295</v>
+      </c>
+      <c r="B58" t="s">
+        <v>267</v>
+      </c>
+      <c r="C58" s="12" t="s">
+        <v>205</v>
+      </c>
+      <c r="D58" t="s">
+        <v>95</v>
+      </c>
+      <c r="E58" t="s">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="59" spans="1:5">
+      <c r="A59" t="s">
+        <v>295</v>
+      </c>
+      <c r="B59" t="s">
+        <v>268</v>
+      </c>
+      <c r="C59" s="12" t="s">
+        <v>205</v>
+      </c>
+      <c r="D59" t="s">
+        <v>95</v>
+      </c>
+      <c r="E59" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="60" spans="1:5">
+      <c r="A60" t="s">
+        <v>295</v>
+      </c>
+      <c r="B60" t="s">
+        <v>269</v>
+      </c>
+      <c r="C60" s="12" t="s">
+        <v>205</v>
+      </c>
+      <c r="D60" t="s">
+        <v>95</v>
+      </c>
+      <c r="E60" t="s">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="61" spans="1:5">
+      <c r="A61" t="s">
+        <v>295</v>
+      </c>
+      <c r="B61" t="s">
+        <v>270</v>
+      </c>
+      <c r="C61" s="12" t="s">
+        <v>205</v>
+      </c>
+      <c r="D61" t="s">
+        <v>95</v>
+      </c>
+      <c r="E61" t="s">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="62" spans="1:5">
+      <c r="A62" t="s">
+        <v>296</v>
+      </c>
+      <c r="B62" t="s">
+        <v>236</v>
+      </c>
+      <c r="C62" s="12" t="s">
+        <v>186</v>
+      </c>
+      <c r="D62" t="s">
+        <v>95</v>
+      </c>
+      <c r="E62" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="63" spans="1:5">
+      <c r="A63" t="s">
+        <v>296</v>
+      </c>
+      <c r="B63" t="s">
+        <v>237</v>
+      </c>
+      <c r="C63" s="12" t="s">
+        <v>187</v>
+      </c>
+      <c r="D63" t="s">
+        <v>95</v>
+      </c>
+      <c r="E63" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="64" spans="1:5">
+      <c r="A64" t="s">
+        <v>296</v>
+      </c>
+      <c r="B64" t="s">
+        <v>238</v>
+      </c>
+      <c r="C64" s="12" t="s">
+        <v>186</v>
+      </c>
+      <c r="D64" t="s">
+        <v>95</v>
+      </c>
+      <c r="E64" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="65" spans="1:5">
+      <c r="A65" t="s">
+        <v>296</v>
+      </c>
+      <c r="B65" t="s">
+        <v>243</v>
+      </c>
+      <c r="C65" s="12" t="s">
+        <v>186</v>
+      </c>
+      <c r="D65" t="s">
+        <v>95</v>
+      </c>
+      <c r="E65" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="66" spans="1:5">
+      <c r="A66" t="s">
+        <v>296</v>
+      </c>
+      <c r="B66" t="s">
+        <v>244</v>
+      </c>
+      <c r="C66" s="12" t="s">
+        <v>186</v>
+      </c>
+      <c r="D66" t="s">
+        <v>95</v>
+      </c>
+      <c r="E66" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="67" spans="1:5">
+      <c r="A67" t="s">
+        <v>296</v>
+      </c>
+      <c r="B67" t="s">
+        <v>239</v>
+      </c>
+      <c r="C67" s="12" t="s">
+        <v>186</v>
+      </c>
+      <c r="D67" t="s">
+        <v>95</v>
+      </c>
+      <c r="E67" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="68" spans="1:5">
+      <c r="A68" t="s">
+        <v>296</v>
+      </c>
+      <c r="B68" t="s">
+        <v>240</v>
+      </c>
+      <c r="C68" s="12" t="s">
+        <v>186</v>
+      </c>
+      <c r="D68" t="s">
+        <v>95</v>
+      </c>
+      <c r="E68" t="s">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="69" spans="1:5">
+      <c r="A69" t="s">
+        <v>296</v>
+      </c>
+      <c r="B69" t="s">
+        <v>245</v>
+      </c>
+      <c r="C69" s="12" t="s">
+        <v>186</v>
+      </c>
+      <c r="D69" t="s">
+        <v>95</v>
+      </c>
+      <c r="E69" t="s">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="70" spans="1:5">
+      <c r="A70" t="s">
+        <v>296</v>
+      </c>
+      <c r="B70" t="s">
+        <v>246</v>
+      </c>
+      <c r="C70" s="12" t="s">
+        <v>186</v>
+      </c>
+      <c r="D70" t="s">
+        <v>95</v>
+      </c>
+      <c r="E70" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="71" spans="1:5">
+      <c r="A71" t="s">
+        <v>296</v>
+      </c>
+      <c r="B71" t="s">
+        <v>241</v>
+      </c>
+      <c r="C71" s="12" t="s">
+        <v>186</v>
+      </c>
+      <c r="D71" t="s">
+        <v>96</v>
+      </c>
+      <c r="E71" t="s">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="72" spans="1:5">
+      <c r="A72" t="s">
+        <v>296</v>
+      </c>
+      <c r="B72" t="s">
+        <v>271</v>
+      </c>
+      <c r="C72" s="12" t="s">
+        <v>186</v>
+      </c>
+      <c r="D72" t="s">
+        <v>142</v>
+      </c>
+      <c r="E72" t="s">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="73" spans="1:5">
+      <c r="A73" t="s">
+        <v>296</v>
+      </c>
+      <c r="B73" t="s">
+        <v>248</v>
+      </c>
+      <c r="C73" s="12" t="s">
+        <v>186</v>
+      </c>
+      <c r="D73" t="s">
+        <v>142</v>
+      </c>
+      <c r="E73" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="74" spans="1:5">
+      <c r="A74" t="s">
+        <v>296</v>
+      </c>
+      <c r="B74" t="s">
+        <v>272</v>
+      </c>
+      <c r="C74" s="12" t="s">
+        <v>186</v>
+      </c>
+      <c r="D74" t="s">
+        <v>142</v>
+      </c>
+      <c r="E74" t="s">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="75" spans="1:5">
+      <c r="A75" t="s">
+        <v>296</v>
+      </c>
+      <c r="B75" t="s">
+        <v>273</v>
+      </c>
+      <c r="C75" s="12" t="s">
+        <v>186</v>
+      </c>
+      <c r="D75" t="s">
+        <v>96</v>
+      </c>
+      <c r="E75" t="s">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="76" spans="1:5">
+      <c r="A76" t="s">
+        <v>297</v>
+      </c>
+      <c r="B76" t="s">
+        <v>274</v>
+      </c>
+      <c r="C76" s="12" t="s">
+        <v>225</v>
+      </c>
+      <c r="D76" t="s">
+        <v>95</v>
+      </c>
+      <c r="E76" t="s">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="77" spans="1:5">
+      <c r="A77" t="s">
+        <v>297</v>
+      </c>
+      <c r="B77" t="s">
+        <v>275</v>
+      </c>
+      <c r="C77" s="12" t="s">
+        <v>225</v>
+      </c>
+      <c r="D77" t="s">
+        <v>95</v>
+      </c>
+      <c r="E77" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="78" spans="1:5">
+      <c r="A78" t="s">
+        <v>297</v>
+      </c>
+      <c r="B78" t="s">
+        <v>238</v>
+      </c>
+      <c r="C78" s="12" t="s">
+        <v>225</v>
+      </c>
+      <c r="D78" t="s">
+        <v>95</v>
+      </c>
+      <c r="E78" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="79" spans="1:5">
+      <c r="A79" t="s">
+        <v>297</v>
+      </c>
+      <c r="B79" t="s">
+        <v>276</v>
+      </c>
+      <c r="C79" s="12" t="s">
+        <v>225</v>
+      </c>
+      <c r="D79" t="s">
+        <v>95</v>
+      </c>
+      <c r="E79" t="s">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="80" spans="1:5">
+      <c r="A80" t="s">
+        <v>297</v>
+      </c>
+      <c r="B80" t="s">
+        <v>277</v>
+      </c>
+      <c r="C80" s="12" t="s">
+        <v>225</v>
+      </c>
+      <c r="D80" t="s">
+        <v>95</v>
+      </c>
+      <c r="E80" t="s">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="81" spans="1:5">
+      <c r="A81" t="s">
+        <v>297</v>
+      </c>
+      <c r="B81" t="s">
+        <v>278</v>
+      </c>
+      <c r="C81" s="12" t="s">
+        <v>225</v>
+      </c>
+      <c r="D81" t="s">
+        <v>95</v>
+      </c>
+      <c r="E81" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="82" spans="1:5">
+      <c r="A82" t="s">
+        <v>297</v>
+      </c>
+      <c r="B82" t="s">
+        <v>279</v>
+      </c>
+      <c r="C82" s="12" t="s">
+        <v>225</v>
+      </c>
+      <c r="D82" t="s">
+        <v>142</v>
+      </c>
+      <c r="E82" t="s">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="83" spans="1:5">
+      <c r="A83" t="s">
+        <v>297</v>
+      </c>
+      <c r="B83" t="s">
+        <v>280</v>
+      </c>
+      <c r="C83" s="12" t="s">
+        <v>225</v>
+      </c>
+      <c r="D83" t="s">
+        <v>95</v>
+      </c>
+      <c r="E83" t="s">
+        <v>232</v>
+      </c>
+    </row>
+    <row r="84" spans="1:5">
+      <c r="A84" t="s">
+        <v>297</v>
+      </c>
+      <c r="B84" t="s">
+        <v>281</v>
+      </c>
+      <c r="C84" s="12" t="s">
+        <v>225</v>
+      </c>
+      <c r="D84" t="s">
+        <v>95</v>
+      </c>
+      <c r="E84" t="s">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="85" spans="1:5">
+      <c r="A85" t="s">
+        <v>297</v>
+      </c>
+      <c r="B85" t="s">
+        <v>236</v>
+      </c>
+      <c r="C85" s="12" t="s">
+        <v>187</v>
+      </c>
+      <c r="D85" t="s">
+        <v>95</v>
+      </c>
+      <c r="E85" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="86" spans="1:5">
+      <c r="A86" t="s">
+        <v>297</v>
+      </c>
+      <c r="B86" t="s">
+        <v>282</v>
+      </c>
+      <c r="C86" s="12" t="s">
+        <v>187</v>
+      </c>
+      <c r="D86" t="s">
+        <v>95</v>
+      </c>
+      <c r="E86" t="s">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="87" spans="1:5">
+      <c r="A87" t="s">
+        <v>297</v>
+      </c>
+      <c r="B87" t="s">
+        <v>283</v>
+      </c>
+      <c r="C87" s="12" t="s">
+        <v>187</v>
+      </c>
+      <c r="D87" t="s">
+        <v>95</v>
+      </c>
+      <c r="E87" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="88" spans="1:5">
+      <c r="A88" t="s">
+        <v>297</v>
+      </c>
+      <c r="B88" t="s">
+        <v>284</v>
+      </c>
+      <c r="C88" s="12" t="s">
+        <v>187</v>
+      </c>
+      <c r="D88" t="s">
+        <v>96</v>
+      </c>
+      <c r="E88" t="s">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="89" spans="1:5">
+      <c r="A89" t="s">
+        <v>297</v>
+      </c>
+      <c r="B89" t="s">
+        <v>285</v>
+      </c>
+      <c r="C89" s="12" t="s">
+        <v>187</v>
+      </c>
+      <c r="D89" t="s">
+        <v>95</v>
+      </c>
+      <c r="E89" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="90" spans="1:5">
+      <c r="A90" t="s">
+        <v>298</v>
+      </c>
+      <c r="B90" t="s">
+        <v>274</v>
+      </c>
+      <c r="C90" s="12" t="s">
+        <v>225</v>
+      </c>
+      <c r="D90" t="s">
+        <v>95</v>
+      </c>
+      <c r="E90" t="s">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="91" spans="1:5">
+      <c r="A91" t="s">
+        <v>298</v>
+      </c>
+      <c r="B91" t="s">
+        <v>275</v>
+      </c>
+      <c r="C91" s="12" t="s">
+        <v>225</v>
+      </c>
+      <c r="D91" t="s">
+        <v>95</v>
+      </c>
+      <c r="E91" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="92" spans="1:5">
+      <c r="A92" t="s">
+        <v>298</v>
+      </c>
+      <c r="B92" t="s">
+        <v>238</v>
+      </c>
+      <c r="C92" s="12" t="s">
+        <v>225</v>
+      </c>
+      <c r="D92" t="s">
+        <v>95</v>
+      </c>
+      <c r="E92" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="93" spans="1:5">
+      <c r="A93" t="s">
+        <v>298</v>
+      </c>
+      <c r="B93" t="s">
+        <v>276</v>
+      </c>
+      <c r="C93" s="12" t="s">
+        <v>225</v>
+      </c>
+      <c r="D93" t="s">
+        <v>95</v>
+      </c>
+      <c r="E93" t="s">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="94" spans="1:5">
+      <c r="A94" t="s">
+        <v>298</v>
+      </c>
+      <c r="B94" t="s">
+        <v>240</v>
+      </c>
+      <c r="C94" s="12" t="s">
+        <v>225</v>
+      </c>
+      <c r="D94" t="s">
+        <v>95</v>
+      </c>
+      <c r="E94" t="s">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="95" spans="1:5">
+      <c r="A95" t="s">
+        <v>298</v>
+      </c>
+      <c r="B95" t="s">
+        <v>277</v>
+      </c>
+      <c r="C95" s="12" t="s">
+        <v>225</v>
+      </c>
+      <c r="D95" t="s">
+        <v>95</v>
+      </c>
+      <c r="E95" t="s">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="96" spans="1:5">
+      <c r="A96" t="s">
+        <v>298</v>
+      </c>
+      <c r="B96" t="s">
+        <v>278</v>
+      </c>
+      <c r="C96" s="12" t="s">
+        <v>225</v>
+      </c>
+      <c r="D96" t="s">
+        <v>95</v>
+      </c>
+      <c r="E96" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="97" spans="1:5">
+      <c r="A97" t="s">
+        <v>298</v>
+      </c>
+      <c r="B97" t="s">
+        <v>279</v>
+      </c>
+      <c r="C97" s="12" t="s">
+        <v>225</v>
+      </c>
+      <c r="D97" t="s">
+        <v>142</v>
+      </c>
+      <c r="E97" t="s">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="98" spans="1:5">
+      <c r="A98" t="s">
+        <v>298</v>
+      </c>
+      <c r="B98" t="s">
+        <v>280</v>
+      </c>
+      <c r="C98" s="12" t="s">
+        <v>225</v>
+      </c>
+      <c r="D98" t="s">
+        <v>95</v>
+      </c>
+      <c r="E98" t="s">
+        <v>232</v>
+      </c>
+    </row>
+    <row r="99" spans="1:5">
+      <c r="A99" t="s">
+        <v>298</v>
+      </c>
+      <c r="B99" t="s">
+        <v>281</v>
+      </c>
+      <c r="C99" s="12" t="s">
+        <v>225</v>
+      </c>
+      <c r="D99" t="s">
+        <v>95</v>
+      </c>
+      <c r="E99" t="s">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="100" spans="1:5">
+      <c r="A100" t="s">
+        <v>298</v>
+      </c>
+      <c r="B100" t="s">
+        <v>236</v>
+      </c>
+      <c r="C100" s="12" t="s">
+        <v>187</v>
+      </c>
+      <c r="D100" t="s">
+        <v>95</v>
+      </c>
+      <c r="E100" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="101" spans="1:5">
+      <c r="A101" t="s">
+        <v>298</v>
+      </c>
+      <c r="B101" t="s">
+        <v>282</v>
+      </c>
+      <c r="C101" s="12" t="s">
+        <v>187</v>
+      </c>
+      <c r="D101" t="s">
+        <v>95</v>
+      </c>
+      <c r="E101" t="s">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="102" spans="1:5">
+      <c r="A102" t="s">
+        <v>298</v>
+      </c>
+      <c r="B102" t="s">
+        <v>283</v>
+      </c>
+      <c r="C102" s="12" t="s">
+        <v>187</v>
+      </c>
+      <c r="D102" t="s">
+        <v>95</v>
+      </c>
+      <c r="E102" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="103" spans="1:5">
+      <c r="A103" t="s">
+        <v>298</v>
+      </c>
+      <c r="B103" t="s">
+        <v>284</v>
+      </c>
+      <c r="C103" s="12" t="s">
+        <v>187</v>
+      </c>
+      <c r="D103" t="s">
+        <v>96</v>
+      </c>
+      <c r="E103" t="s">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="104" spans="1:5">
+      <c r="A104" t="s">
+        <v>298</v>
+      </c>
+      <c r="B104" t="s">
+        <v>285</v>
+      </c>
+      <c r="C104" s="12" t="s">
+        <v>187</v>
+      </c>
+      <c r="D104" t="s">
+        <v>95</v>
+      </c>
+      <c r="E104" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="105" spans="1:5">
+      <c r="A105" t="s">
+        <v>286</v>
+      </c>
+      <c r="D105" t="s">
+        <v>95</v>
+      </c>
+      <c r="E105" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="106" spans="1:5">
+      <c r="A106" t="s">
+        <v>286</v>
+      </c>
+      <c r="D106" t="s">
+        <v>95</v>
+      </c>
+      <c r="E106" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="107" spans="1:5">
+      <c r="A107" t="s">
+        <v>286</v>
+      </c>
+      <c r="D107" t="s">
+        <v>95</v>
+      </c>
+      <c r="E107" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="108" spans="1:5">
+      <c r="A108" t="s">
+        <v>286</v>
+      </c>
+      <c r="D108" t="s">
+        <v>95</v>
+      </c>
+      <c r="E108" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="109" spans="1:5">
+      <c r="A109" t="s">
+        <v>286</v>
+      </c>
+      <c r="D109" t="s">
+        <v>95</v>
+      </c>
+      <c r="E109" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="110" spans="1:5">
+      <c r="A110" t="s">
+        <v>286</v>
+      </c>
+      <c r="D110" t="s">
+        <v>95</v>
+      </c>
+      <c r="E110" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="111" spans="1:5">
+      <c r="A111" t="s">
+        <v>286</v>
+      </c>
+      <c r="D111" t="s">
+        <v>142</v>
+      </c>
+      <c r="E111" t="s">
+        <v>253</v>
+      </c>
+    </row>
+    <row r="112" spans="1:5">
+      <c r="A112" t="s">
+        <v>286</v>
+      </c>
+      <c r="D112" t="s">
+        <v>95</v>
+      </c>
+      <c r="E112" t="s">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="113" spans="1:5">
+      <c r="A113" t="s">
+        <v>286</v>
+      </c>
+      <c r="D113" t="s">
+        <v>95</v>
+      </c>
+      <c r="E113" t="s">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="114" spans="1:5">
+      <c r="A114" t="s">
+        <v>286</v>
+      </c>
+      <c r="D114" t="s">
+        <v>95</v>
+      </c>
+      <c r="E114" t="s">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="115" spans="1:5">
+      <c r="A115" t="s">
+        <v>286</v>
+      </c>
+      <c r="D115" t="s">
+        <v>95</v>
+      </c>
+      <c r="E115" t="s">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="116" spans="1:5">
+      <c r="A116" t="s">
+        <v>286</v>
+      </c>
+      <c r="D116" t="s">
+        <v>95</v>
+      </c>
+      <c r="E116" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="117" spans="1:5">
+      <c r="A117" t="s">
+        <v>286</v>
+      </c>
+      <c r="D117" t="s">
+        <v>142</v>
+      </c>
+      <c r="E117" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="118" spans="1:5">
+      <c r="A118" t="s">
+        <v>286</v>
+      </c>
+      <c r="D118" t="s">
+        <v>96</v>
+      </c>
+      <c r="E118" t="s">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="119" spans="1:5">
+      <c r="A119" t="s">
+        <v>286</v>
+      </c>
+      <c r="D119" t="s">
+        <v>95</v>
+      </c>
+      <c r="E119" t="s">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="120" spans="1:5">
+      <c r="A120" t="s">
+        <v>286</v>
+      </c>
+      <c r="D120" t="s">
+        <v>96</v>
+      </c>
+      <c r="E120" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="121" spans="1:5">
+      <c r="A121" t="s">
+        <v>286</v>
+      </c>
+      <c r="D121" t="s">
+        <v>95</v>
+      </c>
+      <c r="E121" t="s">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="122" spans="1:5">
+      <c r="A122" t="s">
+        <v>286</v>
+      </c>
+      <c r="D122" t="s">
+        <v>95</v>
+      </c>
+      <c r="E122" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="123" spans="1:5">
+      <c r="A123" t="s">
+        <v>286</v>
+      </c>
+      <c r="D123" t="s">
+        <v>96</v>
+      </c>
+      <c r="E123" t="s">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="124" spans="1:5">
+      <c r="A124" t="s">
+        <v>286</v>
+      </c>
+      <c r="D124" t="s">
+        <v>95</v>
+      </c>
+      <c r="E124" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="125" spans="1:5">
+      <c r="A125" t="s">
+        <v>286</v>
+      </c>
+      <c r="D125" t="s">
+        <v>142</v>
+      </c>
+      <c r="E125" t="s">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="126" spans="1:5">
+      <c r="A126" t="s">
+        <v>286</v>
+      </c>
+      <c r="D126" t="s">
+        <v>142</v>
+      </c>
+      <c r="E126" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="127" spans="1:5">
+      <c r="A127" t="s">
+        <v>286</v>
+      </c>
+      <c r="D127" t="s">
+        <v>95</v>
+      </c>
+      <c r="E127" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="128" spans="1:5">
+      <c r="A128" t="s">
+        <v>286</v>
+      </c>
+      <c r="D128" t="s">
+        <v>95</v>
+      </c>
+      <c r="E128" t="s">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="129" spans="1:5">
+      <c r="A129" t="s">
+        <v>286</v>
+      </c>
+      <c r="D129" t="s">
+        <v>95</v>
+      </c>
+      <c r="E129" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="130" spans="1:5">
+      <c r="A130" t="s">
+        <v>286</v>
+      </c>
+      <c r="D130" t="s">
+        <v>95</v>
+      </c>
+      <c r="E130" t="s">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="131" spans="1:5">
+      <c r="A131" t="s">
+        <v>286</v>
+      </c>
+      <c r="D131" t="s">
+        <v>95</v>
+      </c>
+      <c r="E131" t="s">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="132" spans="1:5">
+      <c r="A132" t="s">
+        <v>286</v>
+      </c>
+      <c r="D132" t="s">
+        <v>95</v>
+      </c>
+      <c r="E132" t="s">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="133" spans="1:5">
+      <c r="A133" t="s">
+        <v>286</v>
+      </c>
+      <c r="D133" t="s">
+        <v>95</v>
+      </c>
+      <c r="E133" t="s">
+        <v>301</v>
+      </c>
+    </row>
+    <row r="134" spans="1:5">
+      <c r="A134" t="s">
+        <v>286</v>
+      </c>
+      <c r="D134" t="s">
+        <v>95</v>
+      </c>
+      <c r="E134" t="s">
+        <v>302</v>
+      </c>
+    </row>
+    <row r="135" spans="1:5">
+      <c r="A135" t="s">
+        <v>286</v>
+      </c>
+      <c r="D135" t="s">
+        <v>95</v>
+      </c>
+      <c r="E135" t="s">
+        <v>303</v>
+      </c>
+    </row>
+    <row r="136" spans="1:5">
+      <c r="A136" t="s">
+        <v>286</v>
+      </c>
+      <c r="D136" t="s">
+        <v>95</v>
+      </c>
+      <c r="E136" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="137" spans="1:5">
+      <c r="A137" t="s">
+        <v>286</v>
+      </c>
+      <c r="D137" t="s">
+        <v>95</v>
+      </c>
+      <c r="E137" t="s">
+        <v>306</v>
+      </c>
+    </row>
+    <row r="138" spans="1:5">
+      <c r="A138" t="s">
+        <v>286</v>
+      </c>
+      <c r="D138" t="s">
+        <v>95</v>
+      </c>
+      <c r="E138" t="s">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="139" spans="1:5">
+      <c r="A139" t="s">
+        <v>287</v>
+      </c>
+      <c r="C139" s="12"/>
+      <c r="D139" t="s">
+        <v>95</v>
+      </c>
+      <c r="E139" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="140" spans="1:5">
+      <c r="A140" t="s">
+        <v>287</v>
+      </c>
+      <c r="C140" s="12"/>
+      <c r="D140" t="s">
+        <v>95</v>
+      </c>
+      <c r="E140" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="141" spans="1:5">
+      <c r="A141" t="s">
+        <v>287</v>
+      </c>
+      <c r="C141" s="12"/>
+      <c r="D141" t="s">
+        <v>95</v>
+      </c>
+      <c r="E141" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="142" spans="1:5">
+      <c r="A142" t="s">
+        <v>287</v>
+      </c>
+      <c r="C142" s="12"/>
+      <c r="D142" t="s">
+        <v>95</v>
+      </c>
+      <c r="E142" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="143" spans="1:5">
+      <c r="A143" t="s">
+        <v>287</v>
+      </c>
+      <c r="C143" s="12"/>
+      <c r="D143" t="s">
+        <v>95</v>
+      </c>
+      <c r="E143" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="144" spans="1:5">
+      <c r="A144" t="s">
+        <v>287</v>
+      </c>
+      <c r="C144" s="12"/>
+      <c r="D144" t="s">
+        <v>95</v>
+      </c>
+      <c r="E144" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="145" spans="1:5">
+      <c r="A145" t="s">
+        <v>287</v>
+      </c>
+      <c r="C145" s="12"/>
+      <c r="D145" t="s">
+        <v>95</v>
+      </c>
+      <c r="E145" t="s">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="146" spans="1:5">
+      <c r="A146" t="s">
+        <v>287</v>
+      </c>
+      <c r="C146" s="12"/>
+      <c r="D146" t="s">
+        <v>95</v>
+      </c>
+      <c r="E146" t="s">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="147" spans="1:5">
+      <c r="A147" t="s">
+        <v>287</v>
+      </c>
+      <c r="C147" s="12"/>
+      <c r="D147" t="s">
+        <v>95</v>
+      </c>
+      <c r="E147" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="148" spans="1:5">
+      <c r="A148" t="s">
+        <v>287</v>
+      </c>
+      <c r="C148" s="12"/>
+      <c r="D148" t="s">
+        <v>95</v>
+      </c>
+      <c r="E148" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="149" spans="1:5">
+      <c r="A149" t="s">
+        <v>287</v>
+      </c>
+      <c r="C149" s="12"/>
+      <c r="D149" t="s">
+        <v>96</v>
+      </c>
+      <c r="E149" t="s">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="150" spans="1:5">
+      <c r="A150" t="s">
+        <v>287</v>
+      </c>
+      <c r="C150" s="12"/>
+      <c r="D150" t="s">
+        <v>142</v>
+      </c>
+      <c r="E150" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="151" spans="1:5">
+      <c r="A151" t="s">
+        <v>287</v>
+      </c>
+      <c r="C151" s="12"/>
+      <c r="D151" t="s">
+        <v>142</v>
+      </c>
+      <c r="E151" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="152" spans="1:5">
+      <c r="A152" t="s">
+        <v>287</v>
+      </c>
+      <c r="C152" s="12"/>
+      <c r="D152" t="s">
+        <v>142</v>
+      </c>
+      <c r="E152" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="153" spans="1:5">
+      <c r="A153" t="s">
+        <v>287</v>
+      </c>
+      <c r="C153" s="12"/>
+      <c r="D153" t="s">
+        <v>142</v>
+      </c>
+      <c r="E153" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="154" spans="1:5">
+      <c r="A154" t="s">
+        <v>287</v>
+      </c>
+      <c r="C154" s="12"/>
+      <c r="D154" t="s">
+        <v>142</v>
+      </c>
+      <c r="E154" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="155" spans="1:5">
+      <c r="A155" t="s">
+        <v>287</v>
+      </c>
+      <c r="C155" s="12"/>
+      <c r="D155" t="s">
+        <v>96</v>
+      </c>
+      <c r="E155" t="s">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="156" spans="1:5">
+      <c r="A156" t="s">
+        <v>287</v>
+      </c>
+      <c r="C156" s="12"/>
+      <c r="D156" t="s">
+        <v>95</v>
+      </c>
+      <c r="E156" t="s">
+        <v>299</v>
+      </c>
+    </row>
+    <row r="157" spans="1:5">
+      <c r="A157" t="s">
+        <v>287</v>
+      </c>
+      <c r="C157" s="12"/>
+      <c r="D157" t="s">
+        <v>95</v>
+      </c>
+      <c r="E157" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="158" spans="1:5">
+      <c r="A158" t="s">
+        <v>287</v>
+      </c>
+      <c r="C158" s="12"/>
+      <c r="D158" t="s">
+        <v>95</v>
+      </c>
+      <c r="E158" t="s">
+        <v>306</v>
+      </c>
+    </row>
+    <row r="159" spans="1:5">
+      <c r="A159" t="s">
+        <v>287</v>
+      </c>
+      <c r="C159" s="12"/>
+      <c r="D159" t="s">
+        <v>95</v>
+      </c>
+      <c r="E159" t="s">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="160" spans="1:5">
+      <c r="A160" t="s">
+        <v>311</v>
+      </c>
+      <c r="C160" s="12"/>
+      <c r="D160" t="s">
+        <v>95</v>
+      </c>
+      <c r="E160" t="s">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="161" spans="1:5">
+      <c r="A161" t="s">
+        <v>311</v>
+      </c>
+      <c r="C161" s="12"/>
+      <c r="D161" t="s">
+        <v>95</v>
+      </c>
+      <c r="E161" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="162" spans="1:5">
+      <c r="A162" t="s">
+        <v>311</v>
+      </c>
+      <c r="C162" s="12"/>
+      <c r="D162" t="s">
+        <v>95</v>
+      </c>
+      <c r="E162" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="163" spans="1:5">
+      <c r="A163" t="s">
+        <v>311</v>
+      </c>
+      <c r="C163" s="12"/>
+      <c r="D163" t="s">
+        <v>95</v>
+      </c>
+      <c r="E163" t="s">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="164" spans="1:5">
+      <c r="A164" t="s">
+        <v>311</v>
+      </c>
+      <c r="C164" s="12"/>
+      <c r="D164" t="s">
+        <v>95</v>
+      </c>
+      <c r="E164" t="s">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="165" spans="1:5">
+      <c r="A165" t="s">
+        <v>311</v>
+      </c>
+      <c r="C165" s="12"/>
+      <c r="D165" t="s">
+        <v>95</v>
+      </c>
+      <c r="E165" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="166" spans="1:5">
+      <c r="A166" t="s">
+        <v>311</v>
+      </c>
+      <c r="C166" s="12"/>
+      <c r="D166" t="s">
+        <v>95</v>
+      </c>
+      <c r="E166" t="s">
+        <v>232</v>
+      </c>
+    </row>
+    <row r="167" spans="1:5">
+      <c r="A167" t="s">
+        <v>311</v>
+      </c>
+      <c r="C167" s="12"/>
+      <c r="D167" t="s">
+        <v>95</v>
+      </c>
+      <c r="E167" t="s">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="168" spans="1:5">
+      <c r="A168" t="s">
+        <v>311</v>
+      </c>
+      <c r="C168" s="12"/>
+      <c r="D168" t="s">
+        <v>95</v>
+      </c>
+      <c r="E168" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="169" spans="1:5">
+      <c r="A169" t="s">
+        <v>311</v>
+      </c>
+      <c r="C169" s="12"/>
+      <c r="D169" t="s">
+        <v>95</v>
+      </c>
+      <c r="E169" t="s">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="170" spans="1:5">
+      <c r="A170" t="s">
+        <v>311</v>
+      </c>
+      <c r="C170" s="12"/>
+      <c r="D170" t="s">
+        <v>95</v>
+      </c>
+      <c r="E170" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="171" spans="1:5">
+      <c r="A171" t="s">
+        <v>311</v>
+      </c>
+      <c r="C171" s="12"/>
+      <c r="D171" t="s">
+        <v>96</v>
+      </c>
+      <c r="E171" t="s">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="172" spans="1:5">
+      <c r="A172" t="s">
+        <v>311</v>
+      </c>
+      <c r="C172" s="12"/>
+      <c r="D172" t="s">
+        <v>95</v>
+      </c>
+      <c r="E172" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="173" spans="1:5">
+      <c r="A173" t="s">
+        <v>311</v>
+      </c>
+      <c r="C173" s="12"/>
+      <c r="D173" t="s">
+        <v>95</v>
+      </c>
+      <c r="E173" t="s">
+        <v>304</v>
+      </c>
+    </row>
+    <row r="174" spans="1:5">
+      <c r="A174" t="s">
+        <v>311</v>
+      </c>
+      <c r="C174" s="12"/>
+      <c r="D174" t="s">
+        <v>95</v>
+      </c>
+      <c r="E174" t="s">
+        <v>305</v>
+      </c>
+    </row>
+    <row r="175" spans="1:5">
+      <c r="A175" t="s">
+        <v>311</v>
+      </c>
+      <c r="C175" s="12"/>
+      <c r="D175" t="s">
+        <v>95</v>
+      </c>
+      <c r="E175" t="s">
+        <v>306</v>
+      </c>
+    </row>
+    <row r="176" spans="1:5">
+      <c r="A176" t="s">
+        <v>311</v>
+      </c>
+      <c r="C176" s="12"/>
+      <c r="D176" t="s">
+        <v>142</v>
+      </c>
+      <c r="E176" t="s">
+        <v>310</v>
+      </c>
+    </row>
+    <row r="177" spans="1:5">
+      <c r="A177" t="s">
+        <v>311</v>
+      </c>
+      <c r="C177" s="12"/>
+      <c r="D177" t="s">
+        <v>95</v>
+      </c>
+      <c r="E177" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="178" spans="1:5">
+      <c r="A178" t="s">
+        <v>311</v>
+      </c>
+      <c r="C178" s="12"/>
+      <c r="D178" t="s">
+        <v>95</v>
+      </c>
+      <c r="E178" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="179" spans="1:5">
+      <c r="A179" t="s">
+        <v>311</v>
+      </c>
+      <c r="C179" s="12"/>
+      <c r="D179" t="s">
+        <v>95</v>
+      </c>
+      <c r="E179" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="180" spans="1:5">
+      <c r="A180" t="s">
+        <v>311</v>
+      </c>
+      <c r="C180" s="12"/>
+      <c r="D180" t="s">
+        <v>95</v>
+      </c>
+      <c r="E180" t="s">
+        <v>253</v>
+      </c>
+    </row>
+    <row r="181" spans="1:5">
+      <c r="A181" t="s">
+        <v>311</v>
+      </c>
+      <c r="C181" s="12"/>
+      <c r="D181" t="s">
+        <v>95</v>
+      </c>
+      <c r="E181" t="s">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="182" spans="1:5">
+      <c r="A182" t="s">
+        <v>311</v>
+      </c>
+      <c r="C182" s="12"/>
+      <c r="D182" t="s">
+        <v>142</v>
+      </c>
+      <c r="E182" t="s">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="183" spans="1:5">
+      <c r="A183" t="s">
+        <v>311</v>
+      </c>
+      <c r="C183" s="12"/>
+      <c r="D183" t="s">
+        <v>95</v>
+      </c>
+      <c r="E183" t="s">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="184" spans="1:5">
+      <c r="A184" t="s">
+        <v>311</v>
+      </c>
+      <c r="C184" s="12"/>
+      <c r="D184" t="s">
+        <v>95</v>
+      </c>
+      <c r="E184" t="s">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="185" spans="1:5">
+      <c r="A185" t="s">
+        <v>311</v>
+      </c>
+      <c r="C185" s="12"/>
+      <c r="D185" t="s">
+        <v>95</v>
+      </c>
+      <c r="E185" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="186" spans="1:5">
+      <c r="A186" t="s">
+        <v>311</v>
+      </c>
+      <c r="C186" s="12"/>
+      <c r="D186" t="s">
+        <v>142</v>
+      </c>
+      <c r="E186" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="187" spans="1:5">
+      <c r="A187" t="s">
+        <v>311</v>
+      </c>
+      <c r="C187" s="12"/>
+      <c r="D187" t="s">
+        <v>96</v>
+      </c>
+      <c r="E187" t="s">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="188" spans="1:5">
+      <c r="A188" t="s">
+        <v>311</v>
+      </c>
+      <c r="C188" s="12"/>
+      <c r="D188" t="s">
+        <v>95</v>
+      </c>
+      <c r="E188" t="s">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="189" spans="1:5">
+      <c r="A189" t="s">
+        <v>311</v>
+      </c>
+      <c r="C189" s="12"/>
+      <c r="D189" t="s">
+        <v>96</v>
+      </c>
+      <c r="E189" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="190" spans="1:5">
+      <c r="A190" t="s">
+        <v>311</v>
+      </c>
+      <c r="C190" s="12"/>
+      <c r="D190" t="s">
+        <v>95</v>
+      </c>
+      <c r="E190" t="s">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="191" spans="1:5">
+      <c r="A191" t="s">
+        <v>311</v>
+      </c>
+      <c r="C191" s="12"/>
+      <c r="D191" t="s">
+        <v>95</v>
+      </c>
+      <c r="E191" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="192" spans="1:5">
+      <c r="A192" t="s">
+        <v>311</v>
+      </c>
+      <c r="C192" s="12"/>
+      <c r="D192" t="s">
+        <v>96</v>
+      </c>
+      <c r="E192" t="s">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="193" spans="1:5">
+      <c r="A193" t="s">
+        <v>311</v>
+      </c>
+      <c r="C193" s="12"/>
+      <c r="D193" t="s">
+        <v>95</v>
+      </c>
+      <c r="E193" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="194" spans="1:5">
+      <c r="A194" t="s">
+        <v>311</v>
+      </c>
+      <c r="C194" s="12"/>
+      <c r="D194" t="s">
+        <v>142</v>
+      </c>
+      <c r="E194" t="s">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="195" spans="1:5">
+      <c r="A195" t="s">
+        <v>311</v>
+      </c>
+      <c r="C195" s="12"/>
+      <c r="D195" t="s">
+        <v>142</v>
+      </c>
+      <c r="E195" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="196" spans="1:5">
+      <c r="A196" t="s">
+        <v>311</v>
+      </c>
+      <c r="C196" s="12"/>
+      <c r="D196" t="s">
+        <v>142</v>
+      </c>
+      <c r="E196" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="197" spans="1:5">
+      <c r="A197" t="s">
+        <v>311</v>
+      </c>
+      <c r="C197" s="12"/>
+      <c r="D197" t="s">
+        <v>95</v>
+      </c>
+      <c r="E197" t="s">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="198" spans="1:5">
+      <c r="A198" t="s">
+        <v>311</v>
+      </c>
+      <c r="C198" s="12"/>
+      <c r="D198" t="s">
+        <v>95</v>
+      </c>
+      <c r="E198" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="199" spans="1:5">
+      <c r="A199" t="s">
+        <v>311</v>
+      </c>
+      <c r="C199" s="12"/>
+      <c r="D199" t="s">
+        <v>95</v>
+      </c>
+      <c r="E199" t="s">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="200" spans="1:5">
+      <c r="A200" t="s">
+        <v>311</v>
+      </c>
+      <c r="C200" s="12"/>
+      <c r="D200" t="s">
+        <v>95</v>
+      </c>
+      <c r="E200" t="s">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="201" spans="1:5">
+      <c r="A201" t="s">
+        <v>311</v>
+      </c>
+      <c r="C201" s="12"/>
+      <c r="D201" t="s">
+        <v>95</v>
+      </c>
+      <c r="E201" t="s">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="202" spans="1:5">
+      <c r="A202" t="s">
+        <v>311</v>
+      </c>
+      <c r="C202" s="12"/>
+      <c r="D202" t="s">
+        <v>95</v>
+      </c>
+      <c r="E202" t="s">
+        <v>301</v>
+      </c>
+    </row>
+    <row r="203" spans="1:5">
+      <c r="A203" t="s">
+        <v>311</v>
+      </c>
+      <c r="C203" s="12"/>
+      <c r="D203" t="s">
+        <v>95</v>
+      </c>
+      <c r="E203" t="s">
+        <v>302</v>
+      </c>
+    </row>
+    <row r="204" spans="1:5">
+      <c r="A204" t="s">
+        <v>311</v>
+      </c>
+      <c r="C204" s="12"/>
+      <c r="D204" t="s">
+        <v>95</v>
+      </c>
+      <c r="E204" t="s">
+        <v>303</v>
+      </c>
+    </row>
+    <row r="205" spans="1:5">
+      <c r="A205" t="s">
+        <v>309</v>
+      </c>
+      <c r="C205" s="12"/>
+      <c r="D205" t="s">
+        <v>95</v>
+      </c>
+      <c r="E205" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="206" spans="1:5">
+      <c r="A206" t="s">
+        <v>309</v>
+      </c>
+      <c r="C206" s="12"/>
+      <c r="D206" t="s">
+        <v>143</v>
+      </c>
+      <c r="E206" t="s">
+        <v>312</v>
+      </c>
+    </row>
+    <row r="207" spans="1:5">
+      <c r="A207" t="s">
+        <v>309</v>
+      </c>
+      <c r="C207" s="12"/>
+      <c r="D207" t="s">
+        <v>95</v>
+      </c>
+      <c r="E207" t="s">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="208" spans="1:5">
+      <c r="A208" t="s">
+        <v>309</v>
+      </c>
+      <c r="C208" s="12"/>
+      <c r="D208" t="s">
+        <v>142</v>
+      </c>
+      <c r="E208" t="s">
+        <v>313</v>
+      </c>
+    </row>
+    <row r="209" spans="1:5">
+      <c r="A209" t="s">
+        <v>324</v>
+      </c>
+      <c r="C209" s="12"/>
+      <c r="D209" t="s">
+        <v>95</v>
+      </c>
+      <c r="E209" t="s">
+        <v>322</v>
+      </c>
+    </row>
+    <row r="210" spans="1:5">
+      <c r="A210" t="s">
+        <v>324</v>
+      </c>
+      <c r="C210" s="12"/>
+      <c r="D210" t="s">
+        <v>95</v>
+      </c>
+      <c r="E210" t="s">
+        <v>323</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+  <tableParts count="1">
+    <tablePart r:id="rId1"/>
+  </tableParts>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DF424794-3269-4271-90B8-7AD6608D0FA6}">
+  <dimension ref="A1:Q15"/>
+  <sheetViews>
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="A6" sqref="A6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4"/>
+  <cols>
+    <col min="1" max="1" width="95.21875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="8.5546875" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="137.77734375" customWidth="1"/>
-    <col min="17" max="17" width="48.33203125" customWidth="1"/>
+    <col min="17" max="17" width="48.21875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:17" ht="24" customHeight="1">
@@ -3252,7 +6700,7 @@
       <c r="C1" t="s">
         <v>179</v>
       </c>
-      <c r="Q1" s="13"/>
+      <c r="Q1" s="10"/>
     </row>
     <row r="2" spans="1:17" ht="36.6" customHeight="1">
       <c r="A2" t="s">
@@ -3261,7 +6709,7 @@
       <c r="B2">
         <v>1</v>
       </c>
-      <c r="C2" s="14" t="s">
+      <c r="C2" s="11" t="s">
         <v>180</v>
       </c>
     </row>
@@ -3272,7 +6720,7 @@
       <c r="B3">
         <v>2</v>
       </c>
-      <c r="C3" s="14" t="s">
+      <c r="C3" s="11" t="s">
         <v>181</v>
       </c>
     </row>
@@ -3283,8 +6731,129 @@
       <c r="B4">
         <v>3</v>
       </c>
-      <c r="C4" s="14" t="s">
+      <c r="C4" s="11" t="s">
         <v>182</v>
+      </c>
+    </row>
+    <row r="5" spans="1:17">
+      <c r="A5" t="s">
+        <v>317</v>
+      </c>
+      <c r="B5">
+        <v>1</v>
+      </c>
+      <c r="C5" s="11" t="s">
+        <v>314</v>
+      </c>
+    </row>
+    <row r="6" spans="1:17" ht="28.8">
+      <c r="A6" t="s">
+        <v>318</v>
+      </c>
+      <c r="B6">
+        <v>1</v>
+      </c>
+      <c r="C6" s="11" t="s">
+        <v>315</v>
+      </c>
+    </row>
+    <row r="7" spans="1:17">
+      <c r="A7" t="s">
+        <v>319</v>
+      </c>
+      <c r="B7">
+        <v>1</v>
+      </c>
+      <c r="C7" s="11" t="s">
+        <v>314</v>
+      </c>
+    </row>
+    <row r="8" spans="1:17" ht="28.8">
+      <c r="A8" t="s">
+        <v>320</v>
+      </c>
+      <c r="B8">
+        <v>1</v>
+      </c>
+      <c r="C8" s="11" t="s">
+        <v>316</v>
+      </c>
+    </row>
+    <row r="9" spans="1:17" ht="28.8">
+      <c r="A9" t="s">
+        <v>321</v>
+      </c>
+      <c r="B9">
+        <v>1</v>
+      </c>
+      <c r="C9" s="11" t="s">
+        <v>316</v>
+      </c>
+    </row>
+    <row r="10" spans="1:17" ht="43.2">
+      <c r="A10" t="s">
+        <v>286</v>
+      </c>
+      <c r="B10">
+        <v>1</v>
+      </c>
+      <c r="C10" s="11" t="s">
+        <v>289</v>
+      </c>
+    </row>
+    <row r="11" spans="1:17" ht="43.2">
+      <c r="A11" t="s">
+        <v>287</v>
+      </c>
+      <c r="B11">
+        <v>1</v>
+      </c>
+      <c r="C11" s="11" t="s">
+        <v>288</v>
+      </c>
+    </row>
+    <row r="12" spans="1:17" ht="28.8">
+      <c r="A12" t="s">
+        <v>311</v>
+      </c>
+      <c r="B12">
+        <v>1</v>
+      </c>
+      <c r="C12" s="11" t="s">
+        <v>293</v>
+      </c>
+    </row>
+    <row r="13" spans="1:17" ht="28.8">
+      <c r="A13" t="s">
+        <v>311</v>
+      </c>
+      <c r="B13">
+        <v>2</v>
+      </c>
+      <c r="C13" s="11" t="s">
+        <v>290</v>
+      </c>
+    </row>
+    <row r="14" spans="1:17" ht="28.8">
+      <c r="A14" t="s">
+        <v>309</v>
+      </c>
+      <c r="B14">
+        <v>1</v>
+      </c>
+      <c r="C14" s="11" t="s">
+        <v>291</v>
+      </c>
+    </row>
+    <row r="15" spans="1:17">
+      <c r="A15" t="s">
+        <v>309</v>
+      </c>
+      <c r="B15">
+        <v>2</v>
+      </c>
+      <c r="C15" s="11" t="s">
+        <v>292</v>
       </c>
     </row>
   </sheetData>

</xml_diff>